<commit_message>
new mangrove survey and WQ data
</commit_message>
<xml_diff>
--- a/mma/mma_mangroves_fish.xlsx
+++ b/mma/mma_mangroves_fish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gizmo/Github/emc/mma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BDC206-01DB-2449-9854-856A206C605D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AC4F41-E0B2-F749-986F-72E46203E110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{4D01774F-9620-334E-AEDA-F71C67D39665}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{4D01774F-9620-334E-AEDA-F71C67D39665}"/>
   </bookViews>
   <sheets>
     <sheet name="fish" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2027" uniqueCount="431">
   <si>
     <t>date</t>
   </si>
@@ -1328,6 +1328,12 @@
   </si>
   <si>
     <t>Abudefduf taurus</t>
+  </si>
+  <si>
+    <t>Broad Rock</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -1791,8 +1797,8 @@
   <dimension ref="A1:P1475"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F352" sqref="F352"/>
+      <pane ySplit="1" topLeftCell="A394" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F368" sqref="F368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19719,192 +19725,2661 @@
       </c>
     </row>
     <row r="354" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A354" s="30"/>
+      <c r="A354" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B354" t="s">
+        <v>429</v>
+      </c>
+      <c r="C354" t="s">
+        <v>378</v>
+      </c>
+      <c r="D354">
+        <v>1</v>
+      </c>
+      <c r="F354" t="s">
+        <v>182</v>
+      </c>
+      <c r="G354">
+        <v>2</v>
+      </c>
+      <c r="H354">
+        <v>30</v>
+      </c>
+      <c r="J354" t="str">
+        <f>VLOOKUP(F354,lookups!$A$2:$I$151,2,0)</f>
+        <v>Grunt (juvenile)</v>
+      </c>
+      <c r="K354" t="str">
+        <f>VLOOKUP(F354,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon spp.</v>
+      </c>
+      <c r="L354" t="str">
+        <f>VLOOKUP(F354,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M354" t="str">
+        <f>VLOOKUP(F354,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N354">
+        <f>VLOOKUP(F354,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O354">
+        <f>VLOOKUP(F354,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.1581000000000001</v>
+      </c>
+      <c r="P354">
+        <f t="shared" ref="P354:P405" si="7">N354*G354^O354</f>
+        <v>0.11336697287564686</v>
+      </c>
     </row>
     <row r="355" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A355" s="30"/>
+      <c r="A355" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B355" t="s">
+        <v>429</v>
+      </c>
+      <c r="C355" t="s">
+        <v>378</v>
+      </c>
+      <c r="D355">
+        <v>1</v>
+      </c>
+      <c r="F355" t="s">
+        <v>182</v>
+      </c>
+      <c r="G355">
+        <v>2</v>
+      </c>
+      <c r="H355">
+        <v>10</v>
+      </c>
+      <c r="J355" t="str">
+        <f>VLOOKUP(F355,lookups!$A$2:$I$151,2,0)</f>
+        <v>Grunt (juvenile)</v>
+      </c>
+      <c r="K355" t="str">
+        <f>VLOOKUP(F355,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon spp.</v>
+      </c>
+      <c r="L355" t="str">
+        <f>VLOOKUP(F355,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M355" t="str">
+        <f>VLOOKUP(F355,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N355">
+        <f>VLOOKUP(F355,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O355">
+        <f>VLOOKUP(F355,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.1581000000000001</v>
+      </c>
+      <c r="P355">
+        <f t="shared" si="7"/>
+        <v>0.11336697287564686</v>
+      </c>
     </row>
     <row r="356" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A356" s="30"/>
+      <c r="A356" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B356" t="s">
+        <v>429</v>
+      </c>
+      <c r="C356" t="s">
+        <v>378</v>
+      </c>
+      <c r="D356">
+        <v>1</v>
+      </c>
+      <c r="F356" t="s">
+        <v>182</v>
+      </c>
+      <c r="G356">
+        <v>5</v>
+      </c>
+      <c r="H356">
+        <v>40</v>
+      </c>
+      <c r="J356" t="str">
+        <f>VLOOKUP(F356,lookups!$A$2:$I$151,2,0)</f>
+        <v>Grunt (juvenile)</v>
+      </c>
+      <c r="K356" t="str">
+        <f>VLOOKUP(F356,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon spp.</v>
+      </c>
+      <c r="L356" t="str">
+        <f>VLOOKUP(F356,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M356" t="str">
+        <f>VLOOKUP(F356,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N356">
+        <f>VLOOKUP(F356,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O356">
+        <f>VLOOKUP(F356,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.1581000000000001</v>
+      </c>
+      <c r="P356">
+        <f t="shared" si="7"/>
+        <v>2.0474857678676552</v>
+      </c>
     </row>
     <row r="357" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A357" s="30"/>
+      <c r="A357" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B357" t="s">
+        <v>429</v>
+      </c>
+      <c r="C357" t="s">
+        <v>378</v>
+      </c>
+      <c r="D357">
+        <v>1</v>
+      </c>
+      <c r="F357" t="s">
+        <v>387</v>
+      </c>
+      <c r="G357">
+        <v>15</v>
+      </c>
+      <c r="J357" t="str">
+        <f>VLOOKUP(F357,lookups!$A$2:$I$151,2,0)</f>
+        <v>Gray snapper</v>
+      </c>
+      <c r="K357" t="str">
+        <f>VLOOKUP(F357,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanis griseus</v>
+      </c>
+      <c r="L357" t="str">
+        <f>VLOOKUP(F357,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M357" t="str">
+        <f>VLOOKUP(F357,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N357">
+        <f>VLOOKUP(F357,lookups!$A$2:$I$151,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O357">
+        <f>VLOOKUP(F357,lookups!$A$2:$I$151,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P357">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="358" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A358" s="30"/>
+      <c r="A358" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B358" t="s">
+        <v>429</v>
+      </c>
+      <c r="C358" t="s">
+        <v>378</v>
+      </c>
+      <c r="D358">
+        <v>1</v>
+      </c>
+      <c r="F358" t="s">
+        <v>387</v>
+      </c>
+      <c r="G358">
+        <v>35</v>
+      </c>
+      <c r="J358" t="str">
+        <f>VLOOKUP(F358,lookups!$A$2:$I$151,2,0)</f>
+        <v>Gray snapper</v>
+      </c>
+      <c r="K358" t="str">
+        <f>VLOOKUP(F358,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanis griseus</v>
+      </c>
+      <c r="L358" t="str">
+        <f>VLOOKUP(F358,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M358" t="str">
+        <f>VLOOKUP(F358,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N358">
+        <f>VLOOKUP(F358,lookups!$A$2:$I$151,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O358">
+        <f>VLOOKUP(F358,lookups!$A$2:$I$151,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P358">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="359" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A359" s="30"/>
+      <c r="A359" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B359" t="s">
+        <v>429</v>
+      </c>
+      <c r="C359" t="s">
+        <v>378</v>
+      </c>
+      <c r="D359">
+        <v>1</v>
+      </c>
+      <c r="F359" t="s">
+        <v>387</v>
+      </c>
+      <c r="G359">
+        <v>25</v>
+      </c>
+      <c r="H359">
+        <v>8</v>
+      </c>
+      <c r="J359" t="str">
+        <f>VLOOKUP(F359,lookups!$A$2:$I$151,2,0)</f>
+        <v>Gray snapper</v>
+      </c>
+      <c r="K359" t="str">
+        <f>VLOOKUP(F359,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanis griseus</v>
+      </c>
+      <c r="L359" t="str">
+        <f>VLOOKUP(F359,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M359" t="str">
+        <f>VLOOKUP(F359,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N359">
+        <f>VLOOKUP(F359,lookups!$A$2:$I$151,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O359">
+        <f>VLOOKUP(F359,lookups!$A$2:$I$151,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P359">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="360" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A360" s="30"/>
+      <c r="A360" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B360" t="s">
+        <v>429</v>
+      </c>
+      <c r="C360" t="s">
+        <v>378</v>
+      </c>
+      <c r="D360">
+        <v>1</v>
+      </c>
+      <c r="F360" t="s">
+        <v>387</v>
+      </c>
+      <c r="G360">
+        <v>20</v>
+      </c>
+      <c r="H360">
+        <v>2</v>
+      </c>
+      <c r="J360" t="str">
+        <f>VLOOKUP(F360,lookups!$A$2:$I$151,2,0)</f>
+        <v>Gray snapper</v>
+      </c>
+      <c r="K360" t="str">
+        <f>VLOOKUP(F360,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanis griseus</v>
+      </c>
+      <c r="L360" t="str">
+        <f>VLOOKUP(F360,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M360" t="str">
+        <f>VLOOKUP(F360,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N360">
+        <f>VLOOKUP(F360,lookups!$A$2:$I$151,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O360">
+        <f>VLOOKUP(F360,lookups!$A$2:$I$151,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P360">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="361" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A361" s="30"/>
+      <c r="A361" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B361" t="s">
+        <v>429</v>
+      </c>
+      <c r="C361" t="s">
+        <v>378</v>
+      </c>
+      <c r="D361">
+        <v>1</v>
+      </c>
+      <c r="F361" t="s">
+        <v>387</v>
+      </c>
+      <c r="G361">
+        <v>22</v>
+      </c>
+      <c r="H361">
+        <v>5</v>
+      </c>
+      <c r="J361" t="str">
+        <f>VLOOKUP(F361,lookups!$A$2:$I$151,2,0)</f>
+        <v>Gray snapper</v>
+      </c>
+      <c r="K361" t="str">
+        <f>VLOOKUP(F361,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanis griseus</v>
+      </c>
+      <c r="L361" t="str">
+        <f>VLOOKUP(F361,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M361" t="str">
+        <f>VLOOKUP(F361,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N361">
+        <f>VLOOKUP(F361,lookups!$A$2:$I$151,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O361">
+        <f>VLOOKUP(F361,lookups!$A$2:$I$151,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P361">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="362" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A362" s="30"/>
+      <c r="A362" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B362" t="s">
+        <v>429</v>
+      </c>
+      <c r="C362" t="s">
+        <v>378</v>
+      </c>
+      <c r="D362">
+        <v>1</v>
+      </c>
+      <c r="F362" t="s">
+        <v>416</v>
+      </c>
+      <c r="G362">
+        <v>4</v>
+      </c>
+      <c r="H362">
+        <v>25</v>
+      </c>
+      <c r="J362" t="str">
+        <f>VLOOKUP(F362,lookups!$A$2:$I$151,2,0)</f>
+        <v>Hardhead silverside</v>
+      </c>
+      <c r="K362" t="str">
+        <f>VLOOKUP(F362,lookups!$A$2:$I$151,3,0)</f>
+        <v>Atherinomorus stipes</v>
+      </c>
+      <c r="L362" t="str">
+        <f>VLOOKUP(F362,lookups!$A$2:$I$151,4,0)</f>
+        <v>Atherinidae</v>
+      </c>
+      <c r="M362" t="str">
+        <f>VLOOKUP(F362,lookups!$A$2:$I$151,5,0)</f>
+        <v>Planktivore</v>
+      </c>
+      <c r="N362">
+        <f>VLOOKUP(F362,lookups!$A$2:$I$151,6,0)</f>
+        <v>7.2399999999999999E-3</v>
+      </c>
+      <c r="O362">
+        <f>VLOOKUP(F362,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.21</v>
+      </c>
+      <c r="P362">
+        <f t="shared" si="7"/>
+        <v>0.61994211178569292</v>
+      </c>
     </row>
     <row r="363" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A363" s="30"/>
+      <c r="A363" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B363" t="s">
+        <v>429</v>
+      </c>
+      <c r="C363" t="s">
+        <v>378</v>
+      </c>
+      <c r="D363">
+        <v>1</v>
+      </c>
+      <c r="F363" t="s">
+        <v>330</v>
+      </c>
+      <c r="G363">
+        <v>4</v>
+      </c>
+      <c r="H363">
+        <v>6</v>
+      </c>
+      <c r="I363" t="s">
+        <v>430</v>
+      </c>
+      <c r="J363" t="str">
+        <f>VLOOKUP(F363,lookups!$A$2:$I$151,2,0)</f>
+        <v>Redband Parrotfish</v>
+      </c>
+      <c r="K363" t="str">
+        <f>VLOOKUP(F363,lookups!$A$2:$I$151,3,0)</f>
+        <v>Sparisoma aurofrenatum</v>
+      </c>
+      <c r="L363" t="str">
+        <f>VLOOKUP(F363,lookups!$A$2:$I$151,4,0)</f>
+        <v>Scaridae</v>
+      </c>
+      <c r="M363" t="str">
+        <f>VLOOKUP(F363,lookups!$A$2:$I$151,5,0)</f>
+        <v>Herbivores</v>
+      </c>
+      <c r="N363">
+        <f>VLOOKUP(F363,lookups!$A$2:$I$151,6,0)</f>
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="O363">
+        <f>VLOOKUP(F363,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.4291</v>
+      </c>
+      <c r="P363">
+        <f t="shared" si="7"/>
+        <v>0.53368100802107599</v>
+      </c>
     </row>
     <row r="364" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A364" s="30"/>
+      <c r="A364" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B364" t="s">
+        <v>429</v>
+      </c>
+      <c r="C364" t="s">
+        <v>378</v>
+      </c>
+      <c r="D364">
+        <v>1</v>
+      </c>
+      <c r="F364" t="s">
+        <v>330</v>
+      </c>
+      <c r="G364">
+        <v>6</v>
+      </c>
+      <c r="H364">
+        <v>2</v>
+      </c>
+      <c r="I364" t="s">
+        <v>379</v>
+      </c>
+      <c r="J364" t="str">
+        <f>VLOOKUP(F364,lookups!$A$2:$I$151,2,0)</f>
+        <v>Redband Parrotfish</v>
+      </c>
+      <c r="K364" t="str">
+        <f>VLOOKUP(F364,lookups!$A$2:$I$151,3,0)</f>
+        <v>Sparisoma aurofrenatum</v>
+      </c>
+      <c r="L364" t="str">
+        <f>VLOOKUP(F364,lookups!$A$2:$I$151,4,0)</f>
+        <v>Scaridae</v>
+      </c>
+      <c r="M364" t="str">
+        <f>VLOOKUP(F364,lookups!$A$2:$I$151,5,0)</f>
+        <v>Herbivores</v>
+      </c>
+      <c r="N364">
+        <f>VLOOKUP(F364,lookups!$A$2:$I$151,6,0)</f>
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="O364">
+        <f>VLOOKUP(F364,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.4291</v>
+      </c>
+      <c r="P364">
+        <f t="shared" si="7"/>
+        <v>2.1434644468897606</v>
+      </c>
     </row>
     <row r="365" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A365" s="30"/>
+      <c r="A365" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B365" t="s">
+        <v>429</v>
+      </c>
+      <c r="C365" t="s">
+        <v>378</v>
+      </c>
+      <c r="D365">
+        <v>1</v>
+      </c>
+      <c r="F365" t="s">
+        <v>330</v>
+      </c>
+      <c r="G365">
+        <v>2</v>
+      </c>
+      <c r="H365">
+        <v>5</v>
+      </c>
+      <c r="I365" t="s">
+        <v>379</v>
+      </c>
+      <c r="J365" t="str">
+        <f>VLOOKUP(F365,lookups!$A$2:$I$151,2,0)</f>
+        <v>Redband Parrotfish</v>
+      </c>
+      <c r="K365" t="str">
+        <f>VLOOKUP(F365,lookups!$A$2:$I$151,3,0)</f>
+        <v>Sparisoma aurofrenatum</v>
+      </c>
+      <c r="L365" t="str">
+        <f>VLOOKUP(F365,lookups!$A$2:$I$151,4,0)</f>
+        <v>Scaridae</v>
+      </c>
+      <c r="M365" t="str">
+        <f>VLOOKUP(F365,lookups!$A$2:$I$151,5,0)</f>
+        <v>Herbivores</v>
+      </c>
+      <c r="N365">
+        <f>VLOOKUP(F365,lookups!$A$2:$I$151,6,0)</f>
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="O365">
+        <f>VLOOKUP(F365,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.4291</v>
+      </c>
+      <c r="P365">
+        <f t="shared" si="7"/>
+        <v>4.9547276785883491E-2</v>
+      </c>
     </row>
     <row r="366" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A366" s="30"/>
+      <c r="A366" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B366" t="s">
+        <v>429</v>
+      </c>
+      <c r="C366" t="s">
+        <v>378</v>
+      </c>
+      <c r="D366">
+        <v>1</v>
+      </c>
+      <c r="F366" t="s">
+        <v>342</v>
+      </c>
+      <c r="G366">
+        <v>4</v>
+      </c>
+      <c r="I366" t="s">
+        <v>379</v>
+      </c>
+      <c r="J366" t="str">
+        <f>VLOOKUP(F366,lookups!$A$2:$I$151,2,0)</f>
+        <v>Stoplight Parrotfish</v>
+      </c>
+      <c r="K366" t="str">
+        <f>VLOOKUP(F366,lookups!$A$2:$I$151,3,0)</f>
+        <v>Sparisoma viride</v>
+      </c>
+      <c r="L366" t="str">
+        <f>VLOOKUP(F366,lookups!$A$2:$I$151,4,0)</f>
+        <v>Scaridae</v>
+      </c>
+      <c r="M366" t="str">
+        <f>VLOOKUP(F366,lookups!$A$2:$I$151,5,0)</f>
+        <v>Herbivores</v>
+      </c>
+      <c r="N366">
+        <f>VLOOKUP(F366,lookups!$A$2:$I$151,6,0)</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="O366">
+        <f>VLOOKUP(F366,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.9214000000000002</v>
+      </c>
+      <c r="P366">
+        <f t="shared" si="7"/>
+        <v>1.4348221330880631</v>
+      </c>
     </row>
     <row r="367" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A367" s="30"/>
+      <c r="A367" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B367" t="s">
+        <v>429</v>
+      </c>
+      <c r="C367" t="s">
+        <v>378</v>
+      </c>
+      <c r="D367">
+        <v>1</v>
+      </c>
+      <c r="F367" t="s">
+        <v>342</v>
+      </c>
+      <c r="G367">
+        <v>5</v>
+      </c>
+      <c r="I367" t="s">
+        <v>379</v>
+      </c>
+      <c r="J367" t="str">
+        <f>VLOOKUP(F367,lookups!$A$2:$I$151,2,0)</f>
+        <v>Stoplight Parrotfish</v>
+      </c>
+      <c r="K367" t="str">
+        <f>VLOOKUP(F367,lookups!$A$2:$I$151,3,0)</f>
+        <v>Sparisoma viride</v>
+      </c>
+      <c r="L367" t="str">
+        <f>VLOOKUP(F367,lookups!$A$2:$I$151,4,0)</f>
+        <v>Scaridae</v>
+      </c>
+      <c r="M367" t="str">
+        <f>VLOOKUP(F367,lookups!$A$2:$I$151,5,0)</f>
+        <v>Herbivores</v>
+      </c>
+      <c r="N367">
+        <f>VLOOKUP(F367,lookups!$A$2:$I$151,6,0)</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="O367">
+        <f>VLOOKUP(F367,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.9214000000000002</v>
+      </c>
+      <c r="P367">
+        <f t="shared" si="7"/>
+        <v>2.7536642058777425</v>
+      </c>
     </row>
     <row r="368" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A368" s="30"/>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A369" s="30"/>
-    </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A370" s="30"/>
-    </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A371" s="30"/>
-    </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A372" s="30"/>
-    </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A373" s="30"/>
-    </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A374" s="30"/>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A375" s="30"/>
-    </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A376" s="30"/>
-    </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A377" s="30"/>
-    </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A378" s="30"/>
-    </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A379" s="30"/>
-    </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A380" s="30"/>
-    </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A381" s="30"/>
-    </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A382" s="30"/>
-    </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A383" s="30"/>
-    </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A384" s="30"/>
-    </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A385" s="30"/>
-    </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A386" s="30"/>
-    </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A387" s="30"/>
-    </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A388" s="30"/>
-    </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A389" s="30"/>
-    </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A390" s="30"/>
-    </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A391" s="30"/>
-    </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A392" s="30"/>
-    </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A393" s="30"/>
-    </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A394" s="30"/>
-    </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A395" s="30"/>
-    </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A396" s="30"/>
-    </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A397" s="30"/>
-    </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A398" s="30"/>
-    </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A399" s="30"/>
-    </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A400" s="30"/>
-    </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A401" s="30"/>
-    </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A402" s="30"/>
-    </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A403" s="30"/>
-    </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A404" s="30"/>
-    </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A405" s="30"/>
-    </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A368" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B368" t="s">
+        <v>429</v>
+      </c>
+      <c r="C368" t="s">
+        <v>378</v>
+      </c>
+      <c r="D368">
+        <v>1</v>
+      </c>
+      <c r="F368" t="s">
+        <v>315</v>
+      </c>
+      <c r="G368">
+        <v>5</v>
+      </c>
+      <c r="H368">
+        <v>6</v>
+      </c>
+      <c r="I368" t="s">
+        <v>379</v>
+      </c>
+      <c r="J368" t="str">
+        <f>VLOOKUP(F368,lookups!$A$2:$I$151,2,0)</f>
+        <v>Striped Parrotfish</v>
+      </c>
+      <c r="K368" t="str">
+        <f>VLOOKUP(F368,lookups!$A$2:$I$151,3,0)</f>
+        <v>Scarus iserti</v>
+      </c>
+      <c r="L368" t="str">
+        <f>VLOOKUP(F368,lookups!$A$2:$I$151,4,0)</f>
+        <v>Scaridae</v>
+      </c>
+      <c r="M368" t="str">
+        <f>VLOOKUP(F368,lookups!$A$2:$I$151,5,0)</f>
+        <v>Herbivores</v>
+      </c>
+      <c r="N368">
+        <f>VLOOKUP(F368,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.47E-2</v>
+      </c>
+      <c r="O368">
+        <f>VLOOKUP(F368,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.0548000000000002</v>
+      </c>
+      <c r="P368">
+        <f t="shared" si="7"/>
+        <v>2.0069238957862789</v>
+      </c>
+    </row>
+    <row r="369" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A369" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B369" t="s">
+        <v>429</v>
+      </c>
+      <c r="C369" t="s">
+        <v>378</v>
+      </c>
+      <c r="D369">
+        <v>1</v>
+      </c>
+      <c r="F369" t="s">
+        <v>315</v>
+      </c>
+      <c r="G369">
+        <v>3</v>
+      </c>
+      <c r="H369">
+        <v>2</v>
+      </c>
+      <c r="I369" t="s">
+        <v>379</v>
+      </c>
+      <c r="J369" t="str">
+        <f>VLOOKUP(F369,lookups!$A$2:$I$151,2,0)</f>
+        <v>Striped Parrotfish</v>
+      </c>
+      <c r="K369" t="str">
+        <f>VLOOKUP(F369,lookups!$A$2:$I$151,3,0)</f>
+        <v>Scarus iserti</v>
+      </c>
+      <c r="L369" t="str">
+        <f>VLOOKUP(F369,lookups!$A$2:$I$151,4,0)</f>
+        <v>Scaridae</v>
+      </c>
+      <c r="M369" t="str">
+        <f>VLOOKUP(F369,lookups!$A$2:$I$151,5,0)</f>
+        <v>Herbivores</v>
+      </c>
+      <c r="N369">
+        <f>VLOOKUP(F369,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.47E-2</v>
+      </c>
+      <c r="O369">
+        <f>VLOOKUP(F369,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.0548000000000002</v>
+      </c>
+      <c r="P369">
+        <f t="shared" si="7"/>
+        <v>0.42152888881536776</v>
+      </c>
+    </row>
+    <row r="370" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A370" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B370" t="s">
+        <v>429</v>
+      </c>
+      <c r="C370" t="s">
+        <v>378</v>
+      </c>
+      <c r="D370">
+        <v>1</v>
+      </c>
+      <c r="F370" t="s">
+        <v>250</v>
+      </c>
+      <c r="G370">
+        <v>30</v>
+      </c>
+      <c r="J370" t="str">
+        <f>VLOOKUP(F370,lookups!$A$2:$I$151,2,0)</f>
+        <v>Dog Snapper</v>
+      </c>
+      <c r="K370" t="str">
+        <f>VLOOKUP(F370,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanus jocu</v>
+      </c>
+      <c r="L370" t="str">
+        <f>VLOOKUP(F370,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M370" t="str">
+        <f>VLOOKUP(F370,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N370">
+        <f>VLOOKUP(F370,lookups!$A$2:$I$151,6,0)</f>
+        <v>3.0800000000000001E-2</v>
+      </c>
+      <c r="O370">
+        <f>VLOOKUP(F370,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.8574000000000002</v>
+      </c>
+      <c r="P370">
+        <f t="shared" si="7"/>
+        <v>512.00828643855084</v>
+      </c>
+    </row>
+    <row r="371" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A371" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B371" t="s">
+        <v>429</v>
+      </c>
+      <c r="C371" t="s">
+        <v>378</v>
+      </c>
+      <c r="D371">
+        <v>1</v>
+      </c>
+      <c r="F371" t="s">
+        <v>415</v>
+      </c>
+      <c r="G371">
+        <v>4</v>
+      </c>
+      <c r="H371">
+        <v>80</v>
+      </c>
+      <c r="J371" t="str">
+        <f>VLOOKUP(F371,lookups!$A$2:$I$151,2,0)</f>
+        <v>Reef silverside</v>
+      </c>
+      <c r="K371" t="str">
+        <f>VLOOKUP(F371,lookups!$A$2:$I$151,3,0)</f>
+        <v>Hypoatherina harringtonensis</v>
+      </c>
+      <c r="L371" t="str">
+        <f>VLOOKUP(F371,lookups!$A$2:$I$151,4,0)</f>
+        <v>Atherinidae</v>
+      </c>
+      <c r="M371" t="str">
+        <f>VLOOKUP(F371,lookups!$A$2:$I$151,5,0)</f>
+        <v>Planktivore</v>
+      </c>
+      <c r="N371">
+        <f>VLOOKUP(F371,lookups!$A$2:$I$151,6,0)</f>
+        <v>5.8900000000000003E-3</v>
+      </c>
+      <c r="O371">
+        <f>VLOOKUP(F371,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.14</v>
+      </c>
+      <c r="P371">
+        <f t="shared" si="7"/>
+        <v>0.45770290362155691</v>
+      </c>
+    </row>
+    <row r="372" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A372" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B372" t="s">
+        <v>429</v>
+      </c>
+      <c r="C372" t="s">
+        <v>378</v>
+      </c>
+      <c r="D372">
+        <v>1</v>
+      </c>
+      <c r="F372" t="s">
+        <v>415</v>
+      </c>
+      <c r="G372">
+        <v>3</v>
+      </c>
+      <c r="H372">
+        <v>250</v>
+      </c>
+      <c r="J372" t="str">
+        <f>VLOOKUP(F372,lookups!$A$2:$I$151,2,0)</f>
+        <v>Reef silverside</v>
+      </c>
+      <c r="K372" t="str">
+        <f>VLOOKUP(F372,lookups!$A$2:$I$151,3,0)</f>
+        <v>Hypoatherina harringtonensis</v>
+      </c>
+      <c r="L372" t="str">
+        <f>VLOOKUP(F372,lookups!$A$2:$I$151,4,0)</f>
+        <v>Atherinidae</v>
+      </c>
+      <c r="M372" t="str">
+        <f>VLOOKUP(F372,lookups!$A$2:$I$151,5,0)</f>
+        <v>Planktivore</v>
+      </c>
+      <c r="N372">
+        <f>VLOOKUP(F372,lookups!$A$2:$I$151,6,0)</f>
+        <v>5.8900000000000003E-3</v>
+      </c>
+      <c r="O372">
+        <f>VLOOKUP(F372,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.14</v>
+      </c>
+      <c r="P372">
+        <f t="shared" si="7"/>
+        <v>0.18547100899295971</v>
+      </c>
+    </row>
+    <row r="373" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A373" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B373" t="s">
+        <v>429</v>
+      </c>
+      <c r="C373" t="s">
+        <v>378</v>
+      </c>
+      <c r="D373">
+        <v>1</v>
+      </c>
+      <c r="F373" t="s">
+        <v>339</v>
+      </c>
+      <c r="G373">
+        <v>22</v>
+      </c>
+      <c r="H373">
+        <v>3</v>
+      </c>
+      <c r="I373" t="s">
+        <v>380</v>
+      </c>
+      <c r="J373" t="str">
+        <f>VLOOKUP(F373,lookups!$A$2:$I$151,2,0)</f>
+        <v>Yellowtail parrotfish</v>
+      </c>
+      <c r="K373" t="str">
+        <f>VLOOKUP(F373,lookups!$A$2:$I$151,3,0)</f>
+        <v>Sparisoma rubiprinne</v>
+      </c>
+      <c r="L373" t="str">
+        <f>VLOOKUP(F373,lookups!$A$2:$I$151,4,0)</f>
+        <v>Scaridae</v>
+      </c>
+      <c r="M373" t="str">
+        <f>VLOOKUP(F373,lookups!$A$2:$I$151,5,0)</f>
+        <v>Herbivores</v>
+      </c>
+      <c r="N373">
+        <f>VLOOKUP(F373,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="O373">
+        <f>VLOOKUP(F373,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.0640999999999998</v>
+      </c>
+      <c r="P373">
+        <f t="shared" si="7"/>
+        <v>202.50788349100159</v>
+      </c>
+    </row>
+    <row r="374" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A374" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B374" t="s">
+        <v>429</v>
+      </c>
+      <c r="C374" t="s">
+        <v>378</v>
+      </c>
+      <c r="D374">
+        <v>1</v>
+      </c>
+      <c r="F374" t="s">
+        <v>339</v>
+      </c>
+      <c r="G374">
+        <v>18</v>
+      </c>
+      <c r="H374">
+        <v>2</v>
+      </c>
+      <c r="I374" t="s">
+        <v>380</v>
+      </c>
+      <c r="J374" t="str">
+        <f>VLOOKUP(F374,lookups!$A$2:$I$151,2,0)</f>
+        <v>Yellowtail parrotfish</v>
+      </c>
+      <c r="K374" t="str">
+        <f>VLOOKUP(F374,lookups!$A$2:$I$151,3,0)</f>
+        <v>Sparisoma rubiprinne</v>
+      </c>
+      <c r="L374" t="str">
+        <f>VLOOKUP(F374,lookups!$A$2:$I$151,4,0)</f>
+        <v>Scaridae</v>
+      </c>
+      <c r="M374" t="str">
+        <f>VLOOKUP(F374,lookups!$A$2:$I$151,5,0)</f>
+        <v>Herbivores</v>
+      </c>
+      <c r="N374">
+        <f>VLOOKUP(F374,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="O374">
+        <f>VLOOKUP(F374,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.0640999999999998</v>
+      </c>
+      <c r="P374">
+        <f t="shared" si="7"/>
+        <v>109.49772126152578</v>
+      </c>
+    </row>
+    <row r="375" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A375" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B375" t="s">
+        <v>429</v>
+      </c>
+      <c r="C375" t="s">
+        <v>378</v>
+      </c>
+      <c r="D375">
+        <v>1</v>
+      </c>
+      <c r="F375" t="s">
+        <v>339</v>
+      </c>
+      <c r="G375">
+        <v>12</v>
+      </c>
+      <c r="H375">
+        <v>2</v>
+      </c>
+      <c r="I375" t="s">
+        <v>380</v>
+      </c>
+      <c r="J375" t="str">
+        <f>VLOOKUP(F375,lookups!$A$2:$I$151,2,0)</f>
+        <v>Yellowtail parrotfish</v>
+      </c>
+      <c r="K375" t="str">
+        <f>VLOOKUP(F375,lookups!$A$2:$I$151,3,0)</f>
+        <v>Sparisoma rubiprinne</v>
+      </c>
+      <c r="L375" t="str">
+        <f>VLOOKUP(F375,lookups!$A$2:$I$151,4,0)</f>
+        <v>Scaridae</v>
+      </c>
+      <c r="M375" t="str">
+        <f>VLOOKUP(F375,lookups!$A$2:$I$151,5,0)</f>
+        <v>Herbivores</v>
+      </c>
+      <c r="N375">
+        <f>VLOOKUP(F375,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="O375">
+        <f>VLOOKUP(F375,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.0640999999999998</v>
+      </c>
+      <c r="P375">
+        <f t="shared" si="7"/>
+        <v>31.611409036445199</v>
+      </c>
+    </row>
+    <row r="376" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A376" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B376" t="s">
+        <v>429</v>
+      </c>
+      <c r="C376" t="s">
+        <v>378</v>
+      </c>
+      <c r="D376">
+        <v>1</v>
+      </c>
+      <c r="F376" t="s">
+        <v>182</v>
+      </c>
+      <c r="G376">
+        <v>5</v>
+      </c>
+      <c r="H376">
+        <v>20</v>
+      </c>
+      <c r="J376" t="str">
+        <f>VLOOKUP(F376,lookups!$A$2:$I$151,2,0)</f>
+        <v>Grunt (juvenile)</v>
+      </c>
+      <c r="K376" t="str">
+        <f>VLOOKUP(F376,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon spp.</v>
+      </c>
+      <c r="L376" t="str">
+        <f>VLOOKUP(F376,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M376" t="str">
+        <f>VLOOKUP(F376,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N376">
+        <f>VLOOKUP(F376,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O376">
+        <f>VLOOKUP(F376,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.1581000000000001</v>
+      </c>
+      <c r="P376">
+        <f t="shared" si="7"/>
+        <v>2.0474857678676552</v>
+      </c>
+    </row>
+    <row r="377" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A377" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B377" t="s">
+        <v>429</v>
+      </c>
+      <c r="C377" t="s">
+        <v>378</v>
+      </c>
+      <c r="D377">
+        <v>1</v>
+      </c>
+      <c r="F377" t="s">
+        <v>182</v>
+      </c>
+      <c r="G377">
+        <v>2</v>
+      </c>
+      <c r="H377">
+        <v>20</v>
+      </c>
+      <c r="J377" t="str">
+        <f>VLOOKUP(F377,lookups!$A$2:$I$151,2,0)</f>
+        <v>Grunt (juvenile)</v>
+      </c>
+      <c r="K377" t="str">
+        <f>VLOOKUP(F377,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon spp.</v>
+      </c>
+      <c r="L377" t="str">
+        <f>VLOOKUP(F377,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M377" t="str">
+        <f>VLOOKUP(F377,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N377">
+        <f>VLOOKUP(F377,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O377">
+        <f>VLOOKUP(F377,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.1581000000000001</v>
+      </c>
+      <c r="P377">
+        <f t="shared" si="7"/>
+        <v>0.11336697287564686</v>
+      </c>
+    </row>
+    <row r="378" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A378" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B378" t="s">
+        <v>429</v>
+      </c>
+      <c r="C378" t="s">
+        <v>378</v>
+      </c>
+      <c r="D378">
+        <v>1</v>
+      </c>
+      <c r="F378" t="s">
+        <v>182</v>
+      </c>
+      <c r="G378">
+        <v>4</v>
+      </c>
+      <c r="H378">
+        <v>15</v>
+      </c>
+      <c r="J378" t="str">
+        <f>VLOOKUP(F378,lookups!$A$2:$I$151,2,0)</f>
+        <v>Grunt (juvenile)</v>
+      </c>
+      <c r="K378" t="str">
+        <f>VLOOKUP(F378,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon spp.</v>
+      </c>
+      <c r="L378" t="str">
+        <f>VLOOKUP(F378,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M378" t="str">
+        <f>VLOOKUP(F378,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N378">
+        <f>VLOOKUP(F378,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O378">
+        <f>VLOOKUP(F378,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.1581000000000001</v>
+      </c>
+      <c r="P378">
+        <f t="shared" si="7"/>
+        <v>1.0119740581880039</v>
+      </c>
+    </row>
+    <row r="379" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A379" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B379" t="s">
+        <v>429</v>
+      </c>
+      <c r="C379" t="s">
+        <v>378</v>
+      </c>
+      <c r="D379">
+        <v>1</v>
+      </c>
+      <c r="F379" t="s">
+        <v>179</v>
+      </c>
+      <c r="G379">
+        <v>18</v>
+      </c>
+      <c r="H379">
+        <v>5</v>
+      </c>
+      <c r="J379" t="str">
+        <f>VLOOKUP(F379,lookups!$A$2:$I$151,2,0)</f>
+        <v>Bluestriped Grunt</v>
+      </c>
+      <c r="K379" t="str">
+        <f>VLOOKUP(F379,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon sciurus</v>
+      </c>
+      <c r="L379" t="str">
+        <f>VLOOKUP(F379,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M379" t="str">
+        <f>VLOOKUP(F379,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N379">
+        <f>VLOOKUP(F379,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="O379">
+        <f>VLOOKUP(F379,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.9996</v>
+      </c>
+      <c r="P379">
+        <f t="shared" si="7"/>
+        <v>113.01006799818498</v>
+      </c>
+    </row>
+    <row r="380" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A380" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B380" t="s">
+        <v>429</v>
+      </c>
+      <c r="C380" t="s">
+        <v>378</v>
+      </c>
+      <c r="D380">
+        <v>1</v>
+      </c>
+      <c r="F380" t="s">
+        <v>179</v>
+      </c>
+      <c r="G380">
+        <v>20</v>
+      </c>
+      <c r="J380" t="str">
+        <f>VLOOKUP(F380,lookups!$A$2:$I$151,2,0)</f>
+        <v>Bluestriped Grunt</v>
+      </c>
+      <c r="K380" t="str">
+        <f>VLOOKUP(F380,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon sciurus</v>
+      </c>
+      <c r="L380" t="str">
+        <f>VLOOKUP(F380,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M380" t="str">
+        <f>VLOOKUP(F380,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N380">
+        <f>VLOOKUP(F380,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="O380">
+        <f>VLOOKUP(F380,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.9996</v>
+      </c>
+      <c r="P380">
+        <f t="shared" si="7"/>
+        <v>155.01413632226158</v>
+      </c>
+    </row>
+    <row r="381" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A381" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B381" t="s">
+        <v>429</v>
+      </c>
+      <c r="C381" t="s">
+        <v>378</v>
+      </c>
+      <c r="D381">
+        <v>1</v>
+      </c>
+      <c r="F381" t="s">
+        <v>179</v>
+      </c>
+      <c r="G381">
+        <v>12</v>
+      </c>
+      <c r="J381" t="str">
+        <f>VLOOKUP(F381,lookups!$A$2:$I$151,2,0)</f>
+        <v>Bluestriped Grunt</v>
+      </c>
+      <c r="K381" t="str">
+        <f>VLOOKUP(F381,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon sciurus</v>
+      </c>
+      <c r="L381" t="str">
+        <f>VLOOKUP(F381,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M381" t="str">
+        <f>VLOOKUP(F381,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N381">
+        <f>VLOOKUP(F381,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="O381">
+        <f>VLOOKUP(F381,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.9996</v>
+      </c>
+      <c r="P381">
+        <f t="shared" si="7"/>
+        <v>33.489895745293879</v>
+      </c>
+    </row>
+    <row r="382" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A382" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B382" t="s">
+        <v>429</v>
+      </c>
+      <c r="C382" t="s">
+        <v>378</v>
+      </c>
+      <c r="D382">
+        <v>1</v>
+      </c>
+      <c r="F382" t="s">
+        <v>189</v>
+      </c>
+      <c r="G382">
+        <v>6</v>
+      </c>
+      <c r="J382" t="str">
+        <f>VLOOKUP(F382,lookups!$A$2:$I$151,2,0)</f>
+        <v>Slippery Dick</v>
+      </c>
+      <c r="K382" t="str">
+        <f>VLOOKUP(F382,lookups!$A$2:$I$151,3,0)</f>
+        <v>Halichoeres bivittatus</v>
+      </c>
+      <c r="L382" t="str">
+        <f>VLOOKUP(F382,lookups!$A$2:$I$151,4,0)</f>
+        <v>Labridae</v>
+      </c>
+      <c r="M382" t="str">
+        <f>VLOOKUP(F382,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N382">
+        <f>VLOOKUP(F382,lookups!$A$2:$I$151,6,0)</f>
+        <v>9.3299999999999998E-3</v>
+      </c>
+      <c r="O382">
+        <f>VLOOKUP(F382,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.06</v>
+      </c>
+      <c r="P382">
+        <f t="shared" si="7"/>
+        <v>2.2440083567938895</v>
+      </c>
+    </row>
+    <row r="383" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A383" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B383" t="s">
+        <v>429</v>
+      </c>
+      <c r="C383" t="s">
+        <v>378</v>
+      </c>
+      <c r="D383">
+        <v>1</v>
+      </c>
+      <c r="F383" t="s">
+        <v>189</v>
+      </c>
+      <c r="G383">
+        <v>3</v>
+      </c>
+      <c r="J383" t="str">
+        <f>VLOOKUP(F383,lookups!$A$2:$I$151,2,0)</f>
+        <v>Slippery Dick</v>
+      </c>
+      <c r="K383" t="str">
+        <f>VLOOKUP(F383,lookups!$A$2:$I$151,3,0)</f>
+        <v>Halichoeres bivittatus</v>
+      </c>
+      <c r="L383" t="str">
+        <f>VLOOKUP(F383,lookups!$A$2:$I$151,4,0)</f>
+        <v>Labridae</v>
+      </c>
+      <c r="M383" t="str">
+        <f>VLOOKUP(F383,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N383">
+        <f>VLOOKUP(F383,lookups!$A$2:$I$151,6,0)</f>
+        <v>9.3299999999999998E-3</v>
+      </c>
+      <c r="O383">
+        <f>VLOOKUP(F383,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.06</v>
+      </c>
+      <c r="P383">
+        <f t="shared" si="7"/>
+        <v>0.26907458751730307</v>
+      </c>
+    </row>
+    <row r="384" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A384" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B384" t="s">
+        <v>429</v>
+      </c>
+      <c r="C384" t="s">
+        <v>378</v>
+      </c>
+      <c r="D384">
+        <v>1</v>
+      </c>
+      <c r="F384" t="s">
+        <v>245</v>
+      </c>
+      <c r="G384">
+        <v>12</v>
+      </c>
+      <c r="J384" t="str">
+        <f>VLOOKUP(F384,lookups!$A$2:$I$151,2,0)</f>
+        <v>Schoolmaster Snapper</v>
+      </c>
+      <c r="K384" t="str">
+        <f>VLOOKUP(F384,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanus apodus</v>
+      </c>
+      <c r="L384" t="str">
+        <f>VLOOKUP(F384,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M384" t="str">
+        <f>VLOOKUP(F384,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N384">
+        <f>VLOOKUP(F384,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="O384">
+        <f>VLOOKUP(F384,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.9779</v>
+      </c>
+      <c r="P384">
+        <f t="shared" si="7"/>
+        <v>31.731862411966997</v>
+      </c>
+    </row>
+    <row r="385" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A385" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B385" t="s">
+        <v>429</v>
+      </c>
+      <c r="C385" t="s">
+        <v>378</v>
+      </c>
+      <c r="D385">
+        <v>1</v>
+      </c>
+      <c r="F385" t="s">
+        <v>387</v>
+      </c>
+      <c r="G385">
+        <v>10</v>
+      </c>
+      <c r="H385">
+        <v>3</v>
+      </c>
+      <c r="J385" t="str">
+        <f>VLOOKUP(F385,lookups!$A$2:$I$151,2,0)</f>
+        <v>Gray snapper</v>
+      </c>
+      <c r="K385" t="str">
+        <f>VLOOKUP(F385,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanis griseus</v>
+      </c>
+      <c r="L385" t="str">
+        <f>VLOOKUP(F385,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M385" t="str">
+        <f>VLOOKUP(F385,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N385">
+        <f>VLOOKUP(F385,lookups!$A$2:$I$151,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O385">
+        <f>VLOOKUP(F385,lookups!$A$2:$I$151,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P385">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A386" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B386" t="s">
+        <v>429</v>
+      </c>
+      <c r="C386" t="s">
+        <v>378</v>
+      </c>
+      <c r="D386">
+        <v>1</v>
+      </c>
+      <c r="F386" t="s">
+        <v>387</v>
+      </c>
+      <c r="G386">
+        <v>16</v>
+      </c>
+      <c r="H386">
+        <v>5</v>
+      </c>
+      <c r="J386" t="str">
+        <f>VLOOKUP(F386,lookups!$A$2:$I$151,2,0)</f>
+        <v>Gray snapper</v>
+      </c>
+      <c r="K386" t="str">
+        <f>VLOOKUP(F386,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanis griseus</v>
+      </c>
+      <c r="L386" t="str">
+        <f>VLOOKUP(F386,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M386" t="str">
+        <f>VLOOKUP(F386,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N386">
+        <f>VLOOKUP(F386,lookups!$A$2:$I$151,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O386">
+        <f>VLOOKUP(F386,lookups!$A$2:$I$151,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P386">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A387" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B387" t="s">
+        <v>429</v>
+      </c>
+      <c r="C387" t="s">
+        <v>378</v>
+      </c>
+      <c r="D387">
+        <v>1</v>
+      </c>
+      <c r="F387" t="s">
+        <v>387</v>
+      </c>
+      <c r="G387">
+        <v>15</v>
+      </c>
+      <c r="H387">
+        <v>5</v>
+      </c>
+      <c r="J387" t="str">
+        <f>VLOOKUP(F387,lookups!$A$2:$I$151,2,0)</f>
+        <v>Gray snapper</v>
+      </c>
+      <c r="K387" t="str">
+        <f>VLOOKUP(F387,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanis griseus</v>
+      </c>
+      <c r="L387" t="str">
+        <f>VLOOKUP(F387,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M387" t="str">
+        <f>VLOOKUP(F387,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N387">
+        <f>VLOOKUP(F387,lookups!$A$2:$I$151,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O387">
+        <f>VLOOKUP(F387,lookups!$A$2:$I$151,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P387">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A388" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B388" t="s">
+        <v>429</v>
+      </c>
+      <c r="C388" t="s">
+        <v>378</v>
+      </c>
+      <c r="D388">
+        <v>1</v>
+      </c>
+      <c r="F388" t="s">
+        <v>387</v>
+      </c>
+      <c r="G388">
+        <v>6</v>
+      </c>
+      <c r="H388">
+        <v>3</v>
+      </c>
+      <c r="J388" t="str">
+        <f>VLOOKUP(F388,lookups!$A$2:$I$151,2,0)</f>
+        <v>Gray snapper</v>
+      </c>
+      <c r="K388" t="str">
+        <f>VLOOKUP(F388,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanis griseus</v>
+      </c>
+      <c r="L388" t="str">
+        <f>VLOOKUP(F388,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M388" t="str">
+        <f>VLOOKUP(F388,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N388">
+        <f>VLOOKUP(F388,lookups!$A$2:$I$151,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O388">
+        <f>VLOOKUP(F388,lookups!$A$2:$I$151,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P388">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A389" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B389" t="s">
+        <v>429</v>
+      </c>
+      <c r="C389" t="s">
+        <v>378</v>
+      </c>
+      <c r="D389">
+        <v>1</v>
+      </c>
+      <c r="F389" t="s">
+        <v>35</v>
+      </c>
+      <c r="G389">
+        <v>10</v>
+      </c>
+      <c r="J389" t="str">
+        <f>VLOOKUP(F389,lookups!$A$2:$I$151,2,0)</f>
+        <v>Doctorfish</v>
+      </c>
+      <c r="K389" t="str">
+        <f>VLOOKUP(F389,lookups!$A$2:$I$151,3,0)</f>
+        <v>Acanthurus chirurgus</v>
+      </c>
+      <c r="L389" t="str">
+        <f>VLOOKUP(F389,lookups!$A$2:$I$151,4,0)</f>
+        <v>Acanthuridae</v>
+      </c>
+      <c r="M389" t="str">
+        <f>VLOOKUP(F389,lookups!$A$2:$I$151,5,0)</f>
+        <v>Herbivores</v>
+      </c>
+      <c r="N389">
+        <f>VLOOKUP(F389,lookups!$A$2:$I$151,6,0)</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="O389">
+        <f>VLOOKUP(F389,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.5327999999999999</v>
+      </c>
+      <c r="P389">
+        <f t="shared" si="7"/>
+        <v>13.641432906133977</v>
+      </c>
+    </row>
+    <row r="390" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A390" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B390" t="s">
+        <v>429</v>
+      </c>
+      <c r="C390" t="s">
+        <v>378</v>
+      </c>
+      <c r="D390">
+        <v>1</v>
+      </c>
+      <c r="F390" t="s">
+        <v>14</v>
+      </c>
+      <c r="G390">
+        <v>6</v>
+      </c>
+      <c r="J390" t="str">
+        <f>VLOOKUP(F390,lookups!$A$2:$I$151,2,0)</f>
+        <v>Sergeant Major</v>
+      </c>
+      <c r="K390" t="str">
+        <f>VLOOKUP(F390,lookups!$A$2:$I$151,3,0)</f>
+        <v>Abudefduf saxatilis</v>
+      </c>
+      <c r="L390" t="str">
+        <f>VLOOKUP(F390,lookups!$A$2:$I$151,4,0)</f>
+        <v>Pomacentridae</v>
+      </c>
+      <c r="M390" t="str">
+        <f>VLOOKUP(F390,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N390">
+        <f>VLOOKUP(F390,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="O390">
+        <f>VLOOKUP(F390,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.05</v>
+      </c>
+      <c r="P390">
+        <f t="shared" si="7"/>
+        <v>4.2996460108221886</v>
+      </c>
+    </row>
+    <row r="391" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A391" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B391" t="s">
+        <v>429</v>
+      </c>
+      <c r="C391" t="s">
+        <v>378</v>
+      </c>
+      <c r="D391">
+        <v>1</v>
+      </c>
+      <c r="F391" t="s">
+        <v>170</v>
+      </c>
+      <c r="G391">
+        <v>12</v>
+      </c>
+      <c r="H391">
+        <v>10</v>
+      </c>
+      <c r="J391" t="str">
+        <f>VLOOKUP(F391,lookups!$A$2:$I$151,2,0)</f>
+        <v>French Grunt</v>
+      </c>
+      <c r="K391" t="str">
+        <f>VLOOKUP(F391,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon flavolineatum</v>
+      </c>
+      <c r="L391" t="str">
+        <f>VLOOKUP(F391,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M391" t="str">
+        <f>VLOOKUP(F391,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N391">
+        <f>VLOOKUP(F391,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O391">
+        <f>VLOOKUP(F391,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.1581000000000001</v>
+      </c>
+      <c r="P391">
+        <f t="shared" si="7"/>
+        <v>32.506185853485817</v>
+      </c>
+    </row>
+    <row r="392" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A392" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B392" t="s">
+        <v>429</v>
+      </c>
+      <c r="C392" t="s">
+        <v>378</v>
+      </c>
+      <c r="D392">
+        <v>1</v>
+      </c>
+      <c r="F392" t="s">
+        <v>170</v>
+      </c>
+      <c r="G392">
+        <v>10</v>
+      </c>
+      <c r="H392">
+        <v>5</v>
+      </c>
+      <c r="J392" t="str">
+        <f>VLOOKUP(F392,lookups!$A$2:$I$151,2,0)</f>
+        <v>French Grunt</v>
+      </c>
+      <c r="K392" t="str">
+        <f>VLOOKUP(F392,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon flavolineatum</v>
+      </c>
+      <c r="L392" t="str">
+        <f>VLOOKUP(F392,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M392" t="str">
+        <f>VLOOKUP(F392,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N392">
+        <f>VLOOKUP(F392,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O392">
+        <f>VLOOKUP(F392,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.1581000000000001</v>
+      </c>
+      <c r="P392">
+        <f t="shared" si="7"/>
+        <v>18.276949882608324</v>
+      </c>
+    </row>
+    <row r="393" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A393" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B393" t="s">
+        <v>429</v>
+      </c>
+      <c r="C393" t="s">
+        <v>378</v>
+      </c>
+      <c r="D393">
+        <v>1</v>
+      </c>
+      <c r="F393" t="s">
+        <v>170</v>
+      </c>
+      <c r="G393">
+        <v>15</v>
+      </c>
+      <c r="H393">
+        <v>5</v>
+      </c>
+      <c r="J393" t="str">
+        <f>VLOOKUP(F393,lookups!$A$2:$I$151,2,0)</f>
+        <v>French Grunt</v>
+      </c>
+      <c r="K393" t="str">
+        <f>VLOOKUP(F393,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon flavolineatum</v>
+      </c>
+      <c r="L393" t="str">
+        <f>VLOOKUP(F393,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M393" t="str">
+        <f>VLOOKUP(F393,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N393">
+        <f>VLOOKUP(F393,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O393">
+        <f>VLOOKUP(F393,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.1581000000000001</v>
+      </c>
+      <c r="P393">
+        <f t="shared" si="7"/>
+        <v>65.768437801503794</v>
+      </c>
+    </row>
+    <row r="394" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A394" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B394" t="s">
+        <v>429</v>
+      </c>
+      <c r="C394" t="s">
+        <v>378</v>
+      </c>
+      <c r="D394">
+        <v>1</v>
+      </c>
+      <c r="F394" t="s">
+        <v>170</v>
+      </c>
+      <c r="G394">
+        <v>6</v>
+      </c>
+      <c r="J394" t="str">
+        <f>VLOOKUP(F394,lookups!$A$2:$I$151,2,0)</f>
+        <v>French Grunt</v>
+      </c>
+      <c r="K394" t="str">
+        <f>VLOOKUP(F394,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon flavolineatum</v>
+      </c>
+      <c r="L394" t="str">
+        <f>VLOOKUP(F394,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M394" t="str">
+        <f>VLOOKUP(F394,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N394">
+        <f>VLOOKUP(F394,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O394">
+        <f>VLOOKUP(F394,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.1581000000000001</v>
+      </c>
+      <c r="P394">
+        <f t="shared" si="7"/>
+        <v>3.6415240688494404</v>
+      </c>
+    </row>
+    <row r="395" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A395" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B395" t="s">
+        <v>429</v>
+      </c>
+      <c r="C395" t="s">
+        <v>378</v>
+      </c>
+      <c r="D395">
+        <v>1</v>
+      </c>
+      <c r="F395" t="s">
+        <v>361</v>
+      </c>
+      <c r="G395">
+        <v>5</v>
+      </c>
+      <c r="H395">
+        <v>5</v>
+      </c>
+      <c r="J395" t="str">
+        <f>VLOOKUP(F395,lookups!$A$2:$I$151,2,0)</f>
+        <v>3-spot Damselfish</v>
+      </c>
+      <c r="K395" t="str">
+        <f>VLOOKUP(F395,lookups!$A$2:$I$151,3,0)</f>
+        <v>Stegastes planifrons</v>
+      </c>
+      <c r="L395" t="str">
+        <f>VLOOKUP(F395,lookups!$A$2:$I$151,4,0)</f>
+        <v>Pomacentridae</v>
+      </c>
+      <c r="M395" t="str">
+        <f>VLOOKUP(F395,lookups!$A$2:$I$151,5,0)</f>
+        <v>Omnivores</v>
+      </c>
+      <c r="N395">
+        <f>VLOOKUP(F395,lookups!$A$2:$I$151,6,0)</f>
+        <v>2.188E-2</v>
+      </c>
+      <c r="O395">
+        <f>VLOOKUP(F395,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.96</v>
+      </c>
+      <c r="P395">
+        <f t="shared" si="7"/>
+        <v>2.5644753591955127</v>
+      </c>
+    </row>
+    <row r="396" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A396" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B396" t="s">
+        <v>429</v>
+      </c>
+      <c r="C396" t="s">
+        <v>378</v>
+      </c>
+      <c r="D396">
+        <v>1</v>
+      </c>
+      <c r="F396" t="s">
+        <v>283</v>
+      </c>
+      <c r="G396">
+        <v>13</v>
+      </c>
+      <c r="J396" t="str">
+        <f>VLOOKUP(F396,lookups!$A$2:$I$151,2,0)</f>
+        <v>Yellowtail Snapper</v>
+      </c>
+      <c r="K396" t="str">
+        <f>VLOOKUP(F396,lookups!$A$2:$I$151,3,0)</f>
+        <v>Ocyurus chrysurus</v>
+      </c>
+      <c r="L396" t="str">
+        <f>VLOOKUP(F396,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M396" t="str">
+        <f>VLOOKUP(F396,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N396">
+        <f>VLOOKUP(F396,lookups!$A$2:$I$151,6,0)</f>
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="O396">
+        <f>VLOOKUP(F396,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.718</v>
+      </c>
+      <c r="P396">
+        <f t="shared" si="7"/>
+        <v>43.167118030024227</v>
+      </c>
+    </row>
+    <row r="397" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A397" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B397" t="s">
+        <v>429</v>
+      </c>
+      <c r="C397" t="s">
+        <v>378</v>
+      </c>
+      <c r="D397">
+        <v>1</v>
+      </c>
+      <c r="F397" t="s">
+        <v>182</v>
+      </c>
+      <c r="G397">
+        <v>5</v>
+      </c>
+      <c r="H397">
+        <v>10</v>
+      </c>
+      <c r="J397" t="str">
+        <f>VLOOKUP(F397,lookups!$A$2:$I$151,2,0)</f>
+        <v>Grunt (juvenile)</v>
+      </c>
+      <c r="K397" t="str">
+        <f>VLOOKUP(F397,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon spp.</v>
+      </c>
+      <c r="L397" t="str">
+        <f>VLOOKUP(F397,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M397" t="str">
+        <f>VLOOKUP(F397,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N397">
+        <f>VLOOKUP(F397,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O397">
+        <f>VLOOKUP(F397,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.1581000000000001</v>
+      </c>
+      <c r="P397">
+        <f t="shared" si="7"/>
+        <v>2.0474857678676552</v>
+      </c>
+    </row>
+    <row r="398" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A398" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B398" t="s">
+        <v>429</v>
+      </c>
+      <c r="C398" t="s">
+        <v>378</v>
+      </c>
+      <c r="D398">
+        <v>1</v>
+      </c>
+      <c r="F398" t="s">
+        <v>182</v>
+      </c>
+      <c r="G398">
+        <v>8</v>
+      </c>
+      <c r="H398">
+        <v>10</v>
+      </c>
+      <c r="J398" t="str">
+        <f>VLOOKUP(F398,lookups!$A$2:$I$151,2,0)</f>
+        <v>Grunt (juvenile)</v>
+      </c>
+      <c r="K398" t="str">
+        <f>VLOOKUP(F398,lookups!$A$2:$I$151,3,0)</f>
+        <v>Haemulon spp.</v>
+      </c>
+      <c r="L398" t="str">
+        <f>VLOOKUP(F398,lookups!$A$2:$I$151,4,0)</f>
+        <v>Haemulidae</v>
+      </c>
+      <c r="M398" t="str">
+        <f>VLOOKUP(F398,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N398">
+        <f>VLOOKUP(F398,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O398">
+        <f>VLOOKUP(F398,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.1581000000000001</v>
+      </c>
+      <c r="P398">
+        <f t="shared" si="7"/>
+        <v>9.0334201264139971</v>
+      </c>
+    </row>
+    <row r="399" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A399" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B399" t="s">
+        <v>429</v>
+      </c>
+      <c r="C399" t="s">
+        <v>378</v>
+      </c>
+      <c r="D399">
+        <v>1</v>
+      </c>
+      <c r="F399" t="s">
+        <v>245</v>
+      </c>
+      <c r="G399">
+        <v>10</v>
+      </c>
+      <c r="H399">
+        <v>5</v>
+      </c>
+      <c r="J399" t="str">
+        <f>VLOOKUP(F399,lookups!$A$2:$I$151,2,0)</f>
+        <v>Schoolmaster Snapper</v>
+      </c>
+      <c r="K399" t="str">
+        <f>VLOOKUP(F399,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanus apodus</v>
+      </c>
+      <c r="L399" t="str">
+        <f>VLOOKUP(F399,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M399" t="str">
+        <f>VLOOKUP(F399,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N399">
+        <f>VLOOKUP(F399,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="O399">
+        <f>VLOOKUP(F399,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.9779</v>
+      </c>
+      <c r="P399">
+        <f t="shared" si="7"/>
+        <v>18.437487119826521</v>
+      </c>
+    </row>
+    <row r="400" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A400" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B400" t="s">
+        <v>429</v>
+      </c>
+      <c r="C400" t="s">
+        <v>378</v>
+      </c>
+      <c r="D400">
+        <v>1</v>
+      </c>
+      <c r="F400" t="s">
+        <v>245</v>
+      </c>
+      <c r="G400">
+        <v>16</v>
+      </c>
+      <c r="J400" t="str">
+        <f>VLOOKUP(F400,lookups!$A$2:$I$151,2,0)</f>
+        <v>Schoolmaster Snapper</v>
+      </c>
+      <c r="K400" t="str">
+        <f>VLOOKUP(F400,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanus apodus</v>
+      </c>
+      <c r="L400" t="str">
+        <f>VLOOKUP(F400,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M400" t="str">
+        <f>VLOOKUP(F400,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N400">
+        <f>VLOOKUP(F400,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="O400">
+        <f>VLOOKUP(F400,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.9779</v>
+      </c>
+      <c r="P400">
+        <f t="shared" si="7"/>
+        <v>74.73957540234322</v>
+      </c>
+    </row>
+    <row r="401" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A401" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B401" t="s">
+        <v>429</v>
+      </c>
+      <c r="C401" t="s">
+        <v>378</v>
+      </c>
+      <c r="D401">
+        <v>1</v>
+      </c>
+      <c r="F401" t="s">
+        <v>245</v>
+      </c>
+      <c r="G401">
+        <v>6</v>
+      </c>
+      <c r="J401" t="str">
+        <f>VLOOKUP(F401,lookups!$A$2:$I$151,2,0)</f>
+        <v>Schoolmaster Snapper</v>
+      </c>
+      <c r="K401" t="str">
+        <f>VLOOKUP(F401,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanus apodus</v>
+      </c>
+      <c r="L401" t="str">
+        <f>VLOOKUP(F401,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M401" t="str">
+        <f>VLOOKUP(F401,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N401">
+        <f>VLOOKUP(F401,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="O401">
+        <f>VLOOKUP(F401,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.9779</v>
+      </c>
+      <c r="P401">
+        <f t="shared" si="7"/>
+        <v>4.0277113463214924</v>
+      </c>
+    </row>
+    <row r="402" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A402" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B402" t="s">
+        <v>429</v>
+      </c>
+      <c r="C402" t="s">
+        <v>378</v>
+      </c>
+      <c r="D402">
+        <v>1</v>
+      </c>
+      <c r="F402" t="s">
+        <v>245</v>
+      </c>
+      <c r="G402">
+        <v>4</v>
+      </c>
+      <c r="J402" t="str">
+        <f>VLOOKUP(F402,lookups!$A$2:$I$151,2,0)</f>
+        <v>Schoolmaster Snapper</v>
+      </c>
+      <c r="K402" t="str">
+        <f>VLOOKUP(F402,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanus apodus</v>
+      </c>
+      <c r="L402" t="str">
+        <f>VLOOKUP(F402,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M402" t="str">
+        <f>VLOOKUP(F402,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N402">
+        <f>VLOOKUP(F402,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="O402">
+        <f>VLOOKUP(F402,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.9779</v>
+      </c>
+      <c r="P402">
+        <f t="shared" si="7"/>
+        <v>1.2041377673694396</v>
+      </c>
+    </row>
+    <row r="403" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A403" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B403" t="s">
+        <v>429</v>
+      </c>
+      <c r="C403" t="s">
+        <v>378</v>
+      </c>
+      <c r="D403">
+        <v>1</v>
+      </c>
+      <c r="F403" t="s">
+        <v>245</v>
+      </c>
+      <c r="G403">
+        <v>12</v>
+      </c>
+      <c r="H403">
+        <v>2</v>
+      </c>
+      <c r="J403" t="str">
+        <f>VLOOKUP(F403,lookups!$A$2:$I$151,2,0)</f>
+        <v>Schoolmaster Snapper</v>
+      </c>
+      <c r="K403" t="str">
+        <f>VLOOKUP(F403,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanus apodus</v>
+      </c>
+      <c r="L403" t="str">
+        <f>VLOOKUP(F403,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M403" t="str">
+        <f>VLOOKUP(F403,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N403">
+        <f>VLOOKUP(F403,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="O403">
+        <f>VLOOKUP(F403,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.9779</v>
+      </c>
+      <c r="P403">
+        <f t="shared" si="7"/>
+        <v>31.731862411966997</v>
+      </c>
+    </row>
+    <row r="404" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A404" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B404" t="s">
+        <v>429</v>
+      </c>
+      <c r="C404" t="s">
+        <v>378</v>
+      </c>
+      <c r="D404">
+        <v>1</v>
+      </c>
+      <c r="F404" t="s">
+        <v>245</v>
+      </c>
+      <c r="G404">
+        <v>8</v>
+      </c>
+      <c r="J404" t="str">
+        <f>VLOOKUP(F404,lookups!$A$2:$I$151,2,0)</f>
+        <v>Schoolmaster Snapper</v>
+      </c>
+      <c r="K404" t="str">
+        <f>VLOOKUP(F404,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanus apodus</v>
+      </c>
+      <c r="L404" t="str">
+        <f>VLOOKUP(F404,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M404" t="str">
+        <f>VLOOKUP(F404,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N404">
+        <f>VLOOKUP(F404,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="O404">
+        <f>VLOOKUP(F404,lookups!$A$2:$I$151,7,0)</f>
+        <v>2.9779</v>
+      </c>
+      <c r="P404">
+        <f t="shared" si="7"/>
+        <v>9.4866614495889596</v>
+      </c>
+    </row>
+    <row r="405" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A405" s="30">
+        <v>44680</v>
+      </c>
+      <c r="B405" t="s">
+        <v>429</v>
+      </c>
+      <c r="C405" t="s">
+        <v>378</v>
+      </c>
+      <c r="D405">
+        <v>1</v>
+      </c>
+      <c r="F405" t="s">
+        <v>241</v>
+      </c>
+      <c r="G405">
+        <v>18</v>
+      </c>
+      <c r="J405" t="str">
+        <f>VLOOKUP(F405,lookups!$A$2:$I$151,2,0)</f>
+        <v>Mutton Snapper</v>
+      </c>
+      <c r="K405" t="str">
+        <f>VLOOKUP(F405,lookups!$A$2:$I$151,3,0)</f>
+        <v>Lutjanus analis</v>
+      </c>
+      <c r="L405" t="str">
+        <f>VLOOKUP(F405,lookups!$A$2:$I$151,4,0)</f>
+        <v>Lutjanidae</v>
+      </c>
+      <c r="M405" t="str">
+        <f>VLOOKUP(F405,lookups!$A$2:$I$151,5,0)</f>
+        <v>Carnivores</v>
+      </c>
+      <c r="N405">
+        <f>VLOOKUP(F405,lookups!$A$2:$I$151,6,0)</f>
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="O405">
+        <f>VLOOKUP(F405,lookups!$A$2:$I$151,7,0)</f>
+        <v>3.0112000000000001</v>
+      </c>
+      <c r="P405">
+        <f t="shared" si="7"/>
+        <v>97.586913421522155</v>
+      </c>
+    </row>
+    <row r="406" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A406" s="30"/>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A407" s="30"/>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A408" s="30"/>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A409" s="30"/>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A410" s="30"/>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A411" s="30"/>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A412" s="30"/>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A413" s="30"/>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A414" s="30"/>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A415" s="30"/>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A416" s="30"/>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>